<commit_message>
DA coordinates updated from Marja
</commit_message>
<xml_diff>
--- a/DA_damage.xlsx
+++ b/DA_damage.xlsx
@@ -251,17 +251,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -288,13 +284,10 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -439,54 +432,82 @@
         <v>-79.91373333</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>40.435232</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>-79.9137794596383</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>40.434763</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>-79.9137869977501</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>40.434568</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>-79.9140966771776</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>40.434668</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>-79.9151207932949</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>40.434668</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>-79.9151207932949</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>40.435094</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>-79.9163518926827</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="0" t="n">
+        <v>40.435346</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>-79.9163124785583</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -819,13 +840,13 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3"/>
+      <c r="A51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3"/>
+      <c r="A52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3"/>
+      <c r="A53" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>